<commit_message>
Added data driven approach in Tasks
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/testdata/FreeCRMTestData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SeleniumAutomationFramework\FreeCRMTest\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FBFAD9-C82B-4FAA-B6C7-A1C25489A6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8BB22D-9EF5-4A32-A8BD-BF32E4CB7B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2736" yWindow="1140" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{E9226911-F524-4450-92F0-3D4F45D3C5B2}"/>
+    <workbookView xWindow="2988" yWindow="2100" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{E9226911-F524-4450-92F0-3D4F45D3C5B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
     <sheet name="Deals" sheetId="2" r:id="rId2"/>
+    <sheet name="Tasks" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>firstname</t>
   </si>
@@ -107,6 +108,21 @@
   </si>
   <si>
     <t xml:space="preserve">Silverado Trade </t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Completion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BVC </t>
+  </si>
+  <si>
+    <t>ATCO Lab</t>
+  </si>
+  <si>
+    <t>General Dynamics</t>
   </si>
 </sst>
 </file>
@@ -562,7 +578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CDC2E0A-0597-4C8F-A7A1-12CCFAC96653}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -619,4 +635,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEEEFB29-ADCD-4F28-A0C3-6199C26052AE}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>